<commit_message>
read in growth scores
</commit_message>
<xml_diff>
--- a/INPUT-FILES/OES-TABLES/growth-score-lookup.xlsx
+++ b/INPUT-FILES/OES-TABLES/growth-score-lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/DP4-R/INPUT-FILES/OES-TABLES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866961E1-4A80-C748-85B8-A8F1DC436322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF99554E-1769-2741-9844-A23CD8BE754E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="interview" sheetId="1" r:id="rId1"/>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1337,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2235,7 +2235,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>